<commit_message>
part 4 of demographic functions
</commit_message>
<xml_diff>
--- a/demog functions/References/fertility_ex_solutions.xlsx
+++ b/demog functions/References/fertility_ex_solutions.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ridhikashyap/Dropbox/Teaching/Demography and Population/week4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\personal-improvement\demog functions\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F39EF4-FFB5-DE42-9725-5469B7CE9841}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24260" yWindow="4800" windowWidth="26940" windowHeight="16560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Brazil" sheetId="1" r:id="rId1"/>
     <sheet name="Sweden" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -133,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
     <numFmt numFmtId="165" formatCode="###;\-###;0"/>
@@ -529,24 +523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.296875" customWidth="1"/>
+    <col min="4" max="4" width="30.69921875" customWidth="1"/>
+    <col min="5" max="5" width="33.19921875" customWidth="1"/>
+    <col min="6" max="6" width="31.3984375" customWidth="1"/>
     <col min="7" max="7" width="24.5" customWidth="1"/>
-    <col min="8" max="9" width="29.6640625" customWidth="1"/>
+    <col min="8" max="9" width="29.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -575,12 +569,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>0</v>
       </c>
       <c r="B2" s="15">
         <v>98710.255999999994</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G12" si="0">(A2+A3)/2</f>
@@ -590,43 +587,52 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="15">
         <v>393723.92</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>5</v>
       </c>
       <c r="B4" s="15">
         <v>491465.96</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>10</v>
       </c>
       <c r="B5" s="15">
         <v>490852.08</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>15</v>
       </c>
@@ -637,31 +643,31 @@
         <v>69.400000000000006</v>
       </c>
       <c r="D6">
-        <f>C6 * (100/205)</f>
-        <v>33.853658536585371</v>
+        <f>C6 * (100/105)</f>
+        <v>66.095238095238102</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E12" si="1">B6/$C$17</f>
+        <f>B6/$C$17</f>
         <v>0.97981335999999997</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F12" si="2">(D6 * B6/$C$17)</f>
-        <v>33.170266919024399</v>
+        <f t="shared" ref="F6:F12" si="1">(D6 * B6/$C$17)</f>
+        <v>64.760997318095249</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H12" si="3">D6*E6/1000</f>
-        <v>3.3170266919024395E-2</v>
+        <f t="shared" ref="H6:H12" si="2">D6*E6/1000</f>
+        <v>6.4760997318095245E-2</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I12" si="4">G6*H6</f>
-        <v>0.58047967108292686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I6:I12" si="3">G6*H6</f>
+        <v>1.1333174530666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>20</v>
       </c>
@@ -672,31 +678,31 @@
         <v>109.6</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D12" si="5">C7 * (100/205)</f>
-        <v>53.463414634146339</v>
+        <f t="shared" ref="D7:D13" si="4">C7 * (100/105)</f>
+        <v>104.38095238095237</v>
       </c>
       <c r="E7">
+        <f>B7/$C$17</f>
+        <v>0.97709307999999995</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>0.97709307999999995</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>52.238732472195117</v>
+        <v>101.98990625523807</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.10198990625523807</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="3"/>
-        <v>5.2238732472195119E-2</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="4"/>
-        <v>1.1753714806243902</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.2947728907428564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>25</v>
       </c>
@@ -707,31 +713,31 @@
         <v>92.3</v>
       </c>
       <c r="D8">
-        <f t="shared" si="5"/>
-        <v>45.024390243902438</v>
+        <f t="shared" si="4"/>
+        <v>87.904761904761898</v>
       </c>
       <c r="E8">
+        <f t="shared" ref="E6:E12" si="5">B8/$C$17</f>
+        <v>0.97395421999999998</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>0.97395421999999998</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>43.851694880975607</v>
+        <v>85.615213815238093</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
       <c r="H8">
+        <f t="shared" si="2"/>
+        <v>8.5615213815238095E-2</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="3"/>
-        <v>4.3851694880975609E-2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="4"/>
-        <v>1.2059216092268292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.3544183799190477</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>30</v>
       </c>
@@ -742,31 +748,31 @@
         <v>57.4</v>
       </c>
       <c r="D9">
+        <f t="shared" si="4"/>
+        <v>54.666666666666664</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="E9">
+        <v>0.96989154</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>0.96989154</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>27.15696312</v>
+        <v>53.020737520000004</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
       <c r="H9">
+        <f t="shared" si="2"/>
+        <v>5.302073752E-2</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="3"/>
-        <v>2.7156963119999999E-2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="4"/>
-        <v>0.88260130139999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.7231739693999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>35</v>
       </c>
@@ -777,31 +783,31 @@
         <v>30.5</v>
       </c>
       <c r="D10">
+        <f t="shared" si="4"/>
+        <v>29.047619047619047</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="5"/>
-        <v>14.878048780487804</v>
-      </c>
-      <c r="E10">
+        <v>0.96414526</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="1"/>
-        <v>0.96414526</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>14.344600209756097</v>
+        <v>28.006124219047621</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2.8006124219047621E-2</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="3"/>
-        <v>1.4344600209756097E-2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>0.53792250786585361</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.0502296582142858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>40</v>
       </c>
@@ -812,31 +818,31 @@
         <v>10.8</v>
       </c>
       <c r="D11">
+        <f t="shared" si="4"/>
+        <v>10.285714285714286</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="5"/>
-        <v>5.2682926829268295</v>
-      </c>
-      <c r="E11">
+        <v>0.95612052000000003</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>0.95612052000000003</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>5.0371227395121956</v>
+        <v>9.8343824914285722</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>42.5</v>
       </c>
       <c r="H11">
+        <f t="shared" si="2"/>
+        <v>9.8343824914285723E-3</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="3"/>
-        <v>5.0371227395121952E-3</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>0.21407771642926829</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.41796125588571431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>45</v>
       </c>
@@ -847,41 +853,48 @@
         <v>2</v>
       </c>
       <c r="D12">
+        <f t="shared" si="4"/>
+        <v>1.9047619047619047</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="5"/>
-        <v>0.97560975609756095</v>
-      </c>
-      <c r="E12">
+        <v>0.94398424000000003</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>0.94398424000000003</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>0.92096023414634143</v>
+        <v>1.798065219047619</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>47.5</v>
       </c>
       <c r="H12">
+        <f t="shared" si="2"/>
+        <v>1.798065219047619E-3</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="3"/>
-        <v>9.2096023414634139E-4</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>4.3745611121951217E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8.5408097904761907E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>50</v>
       </c>
       <c r="B13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>19</v>
@@ -890,11 +903,11 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -904,41 +917,41 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D21" s="4">
         <f>SUM(C6:C12) * 5 / 1000</f>
         <v>1.86</v>
       </c>
       <c r="E21">
         <f>SUM(D6:D12) * 5/1000</f>
-        <v>0.90731707317073174</v>
+        <v>1.7714285714285716</v>
       </c>
       <c r="F21">
         <f>((SUM(F6:F12)))*5/1000</f>
-        <v>0.88360170287804873</v>
+        <v>1.7251271341904759</v>
       </c>
       <c r="H21">
         <f>SUM(H6:H12) * 5</f>
-        <v>0.88360170287804862</v>
+        <v>1.7251271341904764</v>
       </c>
       <c r="I21">
         <f>SUM(I6:I12)*5/(SUM(H6:H12)*5)</f>
-        <v>26.25685239535823</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>26.256852395358216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>3</v>
       </c>
@@ -949,7 +962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -958,45 +971,45 @@
         <v>0.90731707317073174</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="H24" t="s">
         <v>27</v>
       </c>
       <c r="I24">
         <f>LN(H21)/I21</f>
-        <v>-4.7130127545385531E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.0767940518412093E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="D25" t="s">
         <v>18</v>
       </c>
       <c r="E25">
         <f>D21/F21</f>
-        <v>2.1050208413379554</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.0781814065389528</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="D30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="D31" t="s">
         <v>3</v>
@@ -1006,72 +1019,72 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32" t="s">
         <v>4</v>
       </c>
       <c r="E32">
         <f>E21</f>
-        <v>0.90731707317073174</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+        <v>1.7714285714285716</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="E33">
         <f>F21</f>
-        <v>0.88360170287804873</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+        <v>1.7251271341904759</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="D34" t="s">
         <v>29</v>
       </c>
       <c r="E34">
         <f>E25</f>
-        <v>2.1050208413379554</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+        <v>1.0781814065389528</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="D35" t="s">
         <v>30</v>
       </c>
       <c r="E35">
         <f>I21</f>
-        <v>26.25685239535823</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+        <v>26.256852395358216</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="D36" t="s">
         <v>33</v>
       </c>
       <c r="E36">
         <f>I24</f>
-        <v>-4.7130127545385531E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+        <v>2.0767940518412093E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
     </row>
   </sheetData>
@@ -1080,19 +1093,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C17"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>6</v>
@@ -1123,7 +1136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1183,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1960</v>
       </c>
@@ -1232,7 +1245,7 @@
         <v>27.470414201183431</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1965</v>
       </c>
@@ -1294,7 +1307,7 @@
         <v>27.169284828441508</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1970</v>
       </c>
@@ -1356,7 +1369,7 @@
         <v>26.937564499484001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1975</v>
       </c>
@@ -1418,7 +1431,7 @@
         <v>26.730337078651687</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1980</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>27.577380952380953</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1985</v>
       </c>
@@ -1542,7 +1555,7 @@
         <v>28.369878822850545</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1990</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>28.533231921366724</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1995</v>
       </c>
@@ -1666,7 +1679,7 @@
         <v>29.14989939637827</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>2000</v>
       </c>
@@ -1728,7 +1741,7 @@
         <v>30.350225952227241</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>2005</v>
       </c>
@@ -1790,7 +1803,7 @@
         <v>30.593872623000305</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -1799,7 +1812,7 @@
         <v>2.0234999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>

</xml_diff>